<commit_message>
Herausforderungen Ausgewertet und Interpretiert
</commit_message>
<xml_diff>
--- a/02_Dokumente/Charts.xlsx
+++ b/02_Dokumente/Charts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DominicSchmitz\ownCloud\Documents\Masterthesis\Masterarbeit\02_Dokumente\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB720FAB-7D18-4669-8C1D-6946DF4C992B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46FF10BA-9BA9-455C-BF83-3E23CB3931FF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CF711C2A-8DA6-4990-BDE7-4A7F458A2EE2}"/>
   </bookViews>
@@ -97,6 +97,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF6DF836"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -142,8 +147,15 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE"/>
-              <a:t>Startup</a:t>
+              <a:rPr lang="de-DE">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Start-up</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -192,7 +204,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="00B050"/>
+              <a:srgbClr val="6DF836"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -201,6 +213,47 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1F103A48-387C-49F6-860C-2BDFA6DAFB7E}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[DATENREIHENNAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{4EA10CBF-5556-47D7-8251-8EC756971913}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[WERT]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-A4D7-43EF-AB9E-4925EC40C8DC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -272,7 +325,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -291,7 +344,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FFC000"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -305,15 +358,61 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="FFC000"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
               </a:ln>
               <a:effectLst/>
             </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{00000001-A4D7-43EF-AB9E-4925EC40C8DC}"/>
+              </c:ext>
+            </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{763375D7-E631-46D9-AC2A-63B74F0270FF}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[DATENREIHENNAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{B0BED984-3C39-4054-AE9B-BF0DCE2F7ABA}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[WERT]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-A4D7-43EF-AB9E-4925EC40C8DC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -385,7 +484,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>15</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -404,7 +503,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="C00000"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -413,6 +512,47 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FC849DEF-4237-4387-AAF5-1F1612ECBA89}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[DATENREIHENNAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{973F7673-6940-4EB6-9A47-C515DAFC50E0}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[WERT]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-A4D7-43EF-AB9E-4925EC40C8DC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -701,7 +841,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE"/>
+              <a:rPr lang="de-DE">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Mittelstand</a:t>
             </a:r>
           </a:p>
@@ -751,7 +898,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="00B050"/>
+              <a:srgbClr val="6DF836"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -760,6 +907,47 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{088508CF-9B85-499C-B2BA-FADE06093870}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[DATENREIHENNAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{949F3E6E-94DC-4C95-BA4B-F871E148E1C5}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[WERT]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000003-D79D-44CD-97A4-0FEF1AF6E703}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -831,7 +1019,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -850,7 +1038,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FFC000"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -859,6 +1047,47 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{1A1FFA58-C3D6-43B7-A001-83D9AB6CA8D6}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[DATENREIHENNAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{4F94D3E9-D063-4010-9ED4-1ECE9DCF0F73}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[WERT]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-D79D-44CD-97A4-0FEF1AF6E703}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -930,7 +1159,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>20</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -949,7 +1178,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -963,7 +1192,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="C00000"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -977,6 +1206,47 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D7842423-CB8B-4AB9-A5F6-A63A1C2B4045}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[DATENREIHENNAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{D8F64578-1337-43FB-8AD2-70A59923FC3F}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[WERT]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-6489-474E-8878-578D4F0150E7}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1265,7 +1535,14 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-DE"/>
+              <a:rPr lang="de-DE">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="85000"/>
+                    <a:lumOff val="15000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:rPr>
               <a:t>Konzern</a:t>
             </a:r>
           </a:p>
@@ -1315,7 +1592,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent1"/>
+              <a:srgbClr val="6DF836"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1329,7 +1606,7 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="00B050"/>
+                <a:srgbClr val="6DF836"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -1343,6 +1620,47 @@
             </c:extLst>
           </c:dPt>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{46A4F284-7B34-495D-B82F-DDB5D539AFA7}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[DATENREIHENNAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{3B77EF2A-A3F5-4CBC-96C1-866BAB8C8299}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[WERT]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000005-9909-40BA-8862-6090CD6D62EC}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1433,7 +1751,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="FFC000"/>
+              <a:schemeClr val="accent2"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1442,6 +1760,47 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
+            <c:dLbl>
+              <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{D3A67628-881D-414C-ADF2-46DF5A87ECFA}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[DATENREIHENNAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{175A48D6-45A1-4B9C-B638-E8E247E03AF8}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[WERT]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="1"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000002-7212-49F3-B02F-FE533A1A91C4}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -1532,7 +1891,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="C00000"/>
+              <a:srgbClr val="FF0000"/>
             </a:solidFill>
             <a:ln>
               <a:noFill/>
@@ -1543,6 +1902,29 @@
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
+              <c:tx>
+                <c:rich>
+                  <a:bodyPr/>
+                  <a:lstStyle/>
+                  <a:p>
+                    <a:fld id="{FEFBCB0C-7239-4EA9-885D-1F48763BDCD7}" type="SERIESNAME">
+                      <a:rPr lang="en-US"/>
+                      <a:pPr/>
+                      <a:t>[DATENREIHENNAME]</a:t>
+                    </a:fld>
+                    <a:r>
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:t> </a:t>
+                    </a:r>
+                    <a:fld id="{3B252DC1-311A-4D4F-8FE4-F96DE7642AAF}" type="VALUE">
+                      <a:rPr lang="en-US" baseline="0"/>
+                      <a:pPr/>
+                      <a:t>[WERT]</a:t>
+                    </a:fld>
+                    <a:endParaRPr lang="en-US" baseline="0"/>
+                  </a:p>
+                </c:rich>
+              </c:tx>
               <c:showLegendKey val="0"/>
               <c:showVal val="1"/>
               <c:showCatName val="0"/>
@@ -1550,7 +1932,10 @@
               <c:showPercent val="0"/>
               <c:showBubbleSize val="0"/>
               <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:dlblFieldTable/>
+                  <c15:showDataLabelsRange val="0"/>
+                </c:ext>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000003-9909-40BA-8862-6090CD6D62EC}"/>
                 </c:ext>
@@ -3855,8 +4240,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29967128-78FE-49A6-8C32-29DCB2D5AAA1}">
   <dimension ref="B2:R4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I23" sqref="I23"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3916,10 +4301,10 @@
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
       <c r="B4">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C4">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -3929,10 +4314,10 @@
         <v>45</v>
       </c>
       <c r="H4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J4">
         <v>13</v>

</xml_diff>